<commit_message>
Developed test methods for missed scenarios in merchant portal
</commit_message>
<xml_diff>
--- a/Mobile/coyni_mobile/resources/testdata_merchant.xlsx
+++ b/Mobile/coyni_mobile/resources/testdata_merchant.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\COYNIv_2.3_Merchant\19-apr-2023(Merchant)\coyni-automation\Mobile\coyni_mobile\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48CF2A56-D942-480E-A1B0-BAE4507F0B3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{087A256F-A4EF-416E-828C-B5061654732D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="7" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SignupPage" sheetId="3" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6149" uniqueCount="1111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6260" uniqueCount="1124">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -3208,9 +3208,6 @@
     <t>Sale Order</t>
   </si>
   <si>
-    <t>1-March 2023</t>
-  </si>
-  <si>
     <t>26-March 2023</t>
   </si>
   <si>
@@ -3352,9 +3349,6 @@
     <t>Notifications</t>
   </si>
   <si>
-    <t>Amount entered exceeds your weekly limit</t>
-  </si>
-  <si>
     <t>9987654345</t>
   </si>
   <si>
@@ -3389,6 +3383,51 @@
   </si>
   <si>
     <t>Verify Sale Order Token transaction</t>
+  </si>
+  <si>
+    <t>2-May 2023</t>
+  </si>
+  <si>
+    <t>validateSignUpWithoutPin</t>
+  </si>
+  <si>
+    <t>Verify Sign Up with without set pin</t>
+  </si>
+  <si>
+    <t>Verify sign up with without set pin</t>
+  </si>
+  <si>
+    <t>bicipat11a181dyy@topqte.com</t>
+  </si>
+  <si>
+    <t>507778163</t>
+  </si>
+  <si>
+    <t>login with valid Email and invalid password</t>
+  </si>
+  <si>
+    <t>Admin@</t>
+  </si>
+  <si>
+    <t>Please enter a valid Password</t>
+  </si>
+  <si>
+    <t>Login with Invalid sets of data in Email And Password fields</t>
+  </si>
+  <si>
+    <t>verify login with Invalid sets of data in Email And Password fields</t>
+  </si>
+  <si>
+    <t>abjc@c.co.,abcA@B@,abc.dcom,abc@.com,abc..com,adc@m.c@mm</t>
+  </si>
+  <si>
+    <t>1234567,wwwwwww,YYYYYYY,@#$%^&amp;*,A@fg12f</t>
+  </si>
+  <si>
+    <t>4-May 2023</t>
+  </si>
+  <si>
+    <t>26-April 2023</t>
   </si>
 </sst>
 </file>
@@ -6098,7 +6137,7 @@
         <v>22</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>1102</v>
+        <v>1100</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>24</v>
@@ -6113,7 +6152,7 @@
         <v>336</v>
       </c>
       <c r="J21" s="14" t="s">
-        <v>1103</v>
+        <v>1101</v>
       </c>
       <c r="K21" s="3" t="s">
         <v>24</v>
@@ -6309,7 +6348,7 @@
         <v>620</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="U1" s="21" t="s">
         <v>629</v>
@@ -6422,13 +6461,13 @@
         <v>386</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>24</v>
@@ -6557,13 +6596,13 @@
         <v>386</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>42</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>24</v>
@@ -6700,7 +6739,7 @@
         <v>22</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>24</v>
@@ -6748,7 +6787,7 @@
         <v>42</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>24</v>
@@ -7943,8 +7982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E4E1502-D358-4D5E-A8D8-D1F4207C13D0}">
   <dimension ref="A1:BZ15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D5"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8092,10 +8131,10 @@
         <v>5</v>
       </c>
       <c r="V1" s="21" t="s">
+        <v>1059</v>
+      </c>
+      <c r="W1" s="21" t="s">
         <v>1060</v>
-      </c>
-      <c r="W1" s="21" t="s">
-        <v>1061</v>
       </c>
       <c r="X1" s="21" t="s">
         <v>629</v>
@@ -8134,7 +8173,7 @@
         <v>732</v>
       </c>
       <c r="AJ1" s="21" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="AK1" s="21" t="s">
         <v>728</v>
@@ -8254,13 +8293,13 @@
         <v>1001</v>
       </c>
       <c r="BX1" s="8" t="s">
+        <v>1065</v>
+      </c>
+      <c r="BY1" s="8" t="s">
         <v>1066</v>
       </c>
-      <c r="BY1" s="8" t="s">
-        <v>1067</v>
-      </c>
       <c r="BZ1" s="8" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="2" spans="1:78">
@@ -8268,13 +8307,13 @@
         <v>479</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>24</v>
@@ -8399,13 +8438,13 @@
         <v>479</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>42</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>24</v>
@@ -8538,7 +8577,7 @@
         <v>22</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>24</v>
@@ -8594,7 +8633,7 @@
         <v>42</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>24</v>
@@ -8641,7 +8680,7 @@
         <v>920</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>22</v>
@@ -8686,7 +8725,7 @@
         <v>483</v>
       </c>
       <c r="S6" s="5" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="T6" s="5" t="s">
         <v>684</v>
@@ -8750,7 +8789,7 @@
         <v>920</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>42</v>
@@ -8795,7 +8834,7 @@
         <v>483</v>
       </c>
       <c r="S7" s="5" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="T7" s="5" t="s">
         <v>684</v>
@@ -8859,10 +8898,10 @@
     </row>
     <row r="8" spans="1:78">
       <c r="A8" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="B8" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>22</v>
@@ -8918,10 +8957,10 @@
     </row>
     <row r="9" spans="1:78">
       <c r="A9" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="B9" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>42</v>
@@ -8962,7 +9001,7 @@
         <v>483</v>
       </c>
       <c r="Q9" s="5" t="s">
-        <v>1098</v>
+        <v>393</v>
       </c>
       <c r="R9" s="5" t="s">
         <v>242</v>
@@ -8974,10 +9013,10 @@
     </row>
     <row r="10" spans="1:78" ht="16.5">
       <c r="A10" s="22" t="s">
+        <v>1082</v>
+      </c>
+      <c r="B10" s="22" t="s">
         <v>1083</v>
-      </c>
-      <c r="B10" s="22" t="s">
-        <v>1084</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>22</v>
@@ -9019,7 +9058,7 @@
         <v>483</v>
       </c>
       <c r="S10" s="5" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="T10" s="5" t="s">
         <v>684</v>
@@ -9083,7 +9122,7 @@
         <v>484</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>22</v>
@@ -9191,7 +9230,7 @@
         <v>484</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>42</v>
@@ -9302,10 +9341,10 @@
     </row>
     <row r="13" spans="1:78">
       <c r="A13" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="B13" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>22</v>
@@ -9361,10 +9400,10 @@
     </row>
     <row r="14" spans="1:78">
       <c r="A14" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="B14" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>42</v>
@@ -9417,10 +9456,10 @@
     </row>
     <row r="15" spans="1:78">
       <c r="A15" s="22" t="s">
+        <v>1085</v>
+      </c>
+      <c r="B15" s="22" t="s">
         <v>1086</v>
-      </c>
-      <c r="B15" s="22" t="s">
-        <v>1087</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>22</v>
@@ -10028,10 +10067,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75D61219-69DA-4130-B594-C564417A50F5}">
-  <dimension ref="A1:Z14"/>
+  <dimension ref="A1:AA14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:I2"/>
+      <selection activeCell="AA5" sqref="AA5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10055,9 +10094,10 @@
     <col min="24" max="24" width="28.140625" customWidth="1"/>
     <col min="25" max="25" width="33" customWidth="1"/>
     <col min="26" max="26" width="18.28515625" customWidth="1"/>
+    <col min="27" max="27" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:27">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10136,8 +10176,11 @@
       <c r="Z1" s="8" t="s">
         <v>855</v>
       </c>
-    </row>
-    <row r="2" spans="1:26">
+      <c r="AA1" s="8" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27">
       <c r="A2" t="s">
         <v>521</v>
       </c>
@@ -10199,7 +10242,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="15.75" thickBot="1">
+    <row r="3" spans="1:27" ht="15.75" thickBot="1">
       <c r="A3" t="s">
         <v>521</v>
       </c>
@@ -10262,7 +10305,7 @@
       </c>
       <c r="Y3" s="36"/>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:27">
       <c r="A4" t="s">
         <v>956</v>
       </c>
@@ -10315,7 +10358,7 @@
       <c r="X4" s="5"/>
       <c r="Y4" s="39"/>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:27">
       <c r="A5" t="s">
         <v>528</v>
       </c>
@@ -10370,8 +10413,11 @@
       <c r="R5" s="5" t="s">
         <v>527</v>
       </c>
-    </row>
-    <row r="6" spans="1:26">
+      <c r="AA5" s="5" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27">
       <c r="A6" t="s">
         <v>530</v>
       </c>
@@ -10431,7 +10477,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="7" spans="1:26">
+    <row r="7" spans="1:27">
       <c r="A7" t="s">
         <v>530</v>
       </c>
@@ -10483,7 +10529,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:26">
+    <row r="8" spans="1:27">
       <c r="A8" t="s">
         <v>530</v>
       </c>
@@ -10537,7 +10583,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="9" spans="1:26">
+    <row r="9" spans="1:27">
       <c r="A9" t="s">
         <v>530</v>
       </c>
@@ -10591,7 +10637,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:26">
+    <row r="10" spans="1:27">
       <c r="A10" t="s">
         <v>530</v>
       </c>
@@ -10645,7 +10691,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="15.75" thickBot="1">
+    <row r="11" spans="1:27" ht="15.75" thickBot="1">
       <c r="A11" t="s">
         <v>857</v>
       </c>
@@ -10686,7 +10732,7 @@
         <v>859</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="15.75" thickBot="1">
+    <row r="12" spans="1:27" ht="15.75" thickBot="1">
       <c r="A12" t="s">
         <v>857</v>
       </c>
@@ -10727,7 +10773,7 @@
         <v>859</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="15.75" thickBot="1">
+    <row r="13" spans="1:27" ht="15.75" thickBot="1">
       <c r="A13" t="s">
         <v>857</v>
       </c>
@@ -10768,7 +10814,7 @@
         <v>859</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="15.75" thickBot="1">
+    <row r="14" spans="1:27" ht="15.75" thickBot="1">
       <c r="A14" t="s">
         <v>857</v>
       </c>
@@ -11004,10 +11050,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70C74F6C-F2A6-441A-AC29-0CCBB91534C1}">
-  <dimension ref="A1:U6"/>
+  <dimension ref="A1:V6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:I2"/>
+    <sheetView topLeftCell="R1" zoomScale="119" workbookViewId="0">
+      <selection activeCell="V4" sqref="V4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11026,9 +11072,10 @@
     <col min="17" max="17" width="28.140625" customWidth="1"/>
     <col min="18" max="18" width="26.7109375" customWidth="1"/>
     <col min="19" max="19" width="22.5703125" customWidth="1"/>
+    <col min="22" max="22" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:22">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -11092,8 +11139,11 @@
       <c r="U1" s="8" t="s">
         <v>699</v>
       </c>
-    </row>
-    <row r="2" spans="1:21">
+      <c r="V1" s="8" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22">
       <c r="A2" s="22" t="s">
         <v>548</v>
       </c>
@@ -11154,7 +11204,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:22">
       <c r="A3" s="22" t="s">
         <v>548</v>
       </c>
@@ -11215,7 +11265,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:22">
       <c r="A4" t="s">
         <v>554</v>
       </c>
@@ -11272,8 +11322,11 @@
       </c>
       <c r="S4" s="5"/>
       <c r="T4" s="5"/>
-    </row>
-    <row r="5" spans="1:21">
+      <c r="V4" s="5" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22">
       <c r="A5" t="s">
         <v>556</v>
       </c>
@@ -11329,7 +11382,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="16.5">
+    <row r="6" spans="1:22" ht="16.5">
       <c r="A6" s="22" t="s">
         <v>957</v>
       </c>
@@ -12873,10 +12926,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E611824-810F-4B44-A5CC-5D2A97239559}">
-  <dimension ref="A1:CA6"/>
+  <dimension ref="A1:CB7"/>
   <sheetViews>
-    <sheetView topLeftCell="AO1" workbookViewId="0">
-      <selection activeCell="AV5" sqref="AV5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="CC1" sqref="CC1:CL1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12955,11 +13008,12 @@
     <col min="74" max="74" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="75" max="75" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="76" max="76" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="20.42578125" customWidth="1"/>
-    <col min="79" max="79" width="21.140625" customWidth="1"/>
+    <col min="78" max="78" width="23.85546875" customWidth="1"/>
+    <col min="79" max="79" width="23.42578125" customWidth="1"/>
+    <col min="80" max="80" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:79">
+    <row r="1" spans="1:80">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -13192,13 +13246,16 @@
         <v>1036</v>
       </c>
       <c r="BZ1" s="8" t="s">
-        <v>972</v>
+        <v>1110</v>
       </c>
       <c r="CA1" s="8" t="s">
         <v>968</v>
       </c>
-    </row>
-    <row r="2" spans="1:79">
+      <c r="CB1" s="8" t="s">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="2" spans="1:80">
       <c r="A2" t="s">
         <v>899</v>
       </c>
@@ -13209,7 +13266,7 @@
         <v>22</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>1105</v>
+        <v>1103</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>24</v>
@@ -13365,7 +13422,7 @@
         <v>971</v>
       </c>
       <c r="BD2" s="14" t="s">
-        <v>1106</v>
+        <v>1104</v>
       </c>
       <c r="BE2" s="3" t="s">
         <v>24</v>
@@ -13421,21 +13478,30 @@
       <c r="BV2" s="5" t="s">
         <v>978</v>
       </c>
-    </row>
-    <row r="3" spans="1:79">
+      <c r="BZ2" t="s">
+        <v>127</v>
+      </c>
+      <c r="CA2" s="5" t="s">
+        <v>969</v>
+      </c>
+      <c r="CB2" s="5" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="3" spans="1:80">
       <c r="A3" t="s">
-        <v>901</v>
+        <v>1111</v>
       </c>
       <c r="B3" t="s">
-        <v>900</v>
+        <v>1112</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>928</v>
-      </c>
-      <c r="E3" s="2" t="s">
+        <v>1113</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>24</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -13589,7 +13655,7 @@
         <v>971</v>
       </c>
       <c r="BD3" s="14" t="s">
-        <v>407</v>
+        <v>1114</v>
       </c>
       <c r="BE3" s="3" t="s">
         <v>24</v>
@@ -13639,10 +13705,22 @@
       <c r="BT3" s="5" t="s">
         <v>872</v>
       </c>
-    </row>
-    <row r="4" spans="1:79">
+      <c r="BU3" s="5" t="s">
+        <v>977</v>
+      </c>
+      <c r="BV3" s="5" t="s">
+        <v>978</v>
+      </c>
+      <c r="CA3" s="5" t="s">
+        <v>969</v>
+      </c>
+      <c r="CB3" s="5" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="4" spans="1:80">
       <c r="A4" t="s">
-        <v>1033</v>
+        <v>901</v>
       </c>
       <c r="B4" t="s">
         <v>900</v>
@@ -13651,9 +13729,9 @@
         <v>22</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>1041</v>
-      </c>
-      <c r="E4" s="3" t="s">
+        <v>928</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>24</v>
       </c>
       <c r="F4" s="2" t="s">
@@ -13738,7 +13816,7 @@
         <v>769</v>
       </c>
       <c r="AG4" s="13" t="s">
-        <v>1037</v>
+        <v>784</v>
       </c>
       <c r="AH4" s="35" t="s">
         <v>785</v>
@@ -13857,25 +13935,19 @@
       <c r="BT4" s="5" t="s">
         <v>872</v>
       </c>
-      <c r="BU4" s="5" t="s">
-        <v>977</v>
-      </c>
-      <c r="BV4" s="5" t="s">
-        <v>978</v>
-      </c>
-      <c r="BX4" s="5" t="s">
-        <v>1035</v>
-      </c>
-      <c r="BY4" s="5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="5" spans="1:79">
+      <c r="CA4" s="5" t="s">
+        <v>969</v>
+      </c>
+      <c r="CB4" s="5" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="5" spans="1:80">
       <c r="A5" t="s">
-        <v>1038</v>
+        <v>1033</v>
       </c>
       <c r="B5" t="s">
-        <v>1038</v>
+        <v>900</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>22</v>
@@ -13941,7 +14013,7 @@
         <v>683</v>
       </c>
       <c r="X5" s="13" t="s">
-        <v>1042</v>
+        <v>763</v>
       </c>
       <c r="Y5" s="3" t="s">
         <v>764</v>
@@ -13968,7 +14040,7 @@
         <v>769</v>
       </c>
       <c r="AG5" s="13" t="s">
-        <v>784</v>
+        <v>1037</v>
       </c>
       <c r="AH5" s="35" t="s">
         <v>785</v>
@@ -14037,7 +14109,7 @@
         <v>971</v>
       </c>
       <c r="BD5" s="14" t="s">
-        <v>1032</v>
+        <v>407</v>
       </c>
       <c r="BE5" s="3" t="s">
         <v>24</v>
@@ -14093,25 +14165,31 @@
       <c r="BV5" s="5" t="s">
         <v>978</v>
       </c>
-      <c r="BZ5" s="5" t="s">
-        <v>973</v>
+      <c r="BX5" s="5" t="s">
+        <v>1035</v>
+      </c>
+      <c r="BY5" s="5" t="s">
+        <v>114</v>
       </c>
       <c r="CA5" s="5" t="s">
         <v>969</v>
       </c>
-    </row>
-    <row r="6" spans="1:79">
+      <c r="CB5" s="5" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="6" spans="1:80">
       <c r="A6" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="B6" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>23</v>
+        <v>1041</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>24</v>
@@ -14171,7 +14249,7 @@
         <v>683</v>
       </c>
       <c r="X6" s="13" t="s">
-        <v>763</v>
+        <v>1042</v>
       </c>
       <c r="Y6" s="3" t="s">
         <v>764</v>
@@ -14198,7 +14276,7 @@
         <v>769</v>
       </c>
       <c r="AG6" s="13" t="s">
-        <v>1040</v>
+        <v>784</v>
       </c>
       <c r="AH6" s="35" t="s">
         <v>785</v>
@@ -14267,7 +14345,7 @@
         <v>971</v>
       </c>
       <c r="BD6" s="14" t="s">
-        <v>407</v>
+        <v>1032</v>
       </c>
       <c r="BE6" s="3" t="s">
         <v>24</v>
@@ -14323,11 +14401,247 @@
       <c r="BV6" s="5" t="s">
         <v>978</v>
       </c>
-      <c r="BX6" s="5" t="s">
+      <c r="CA6" s="5" t="s">
+        <v>969</v>
+      </c>
+      <c r="CB6" s="5" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="7" spans="1:80">
+      <c r="A7" t="s">
+        <v>1039</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1039</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>969</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>973</v>
+      </c>
+      <c r="I7" t="s">
+        <v>332</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>576</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>743</v>
+      </c>
+      <c r="L7" t="s">
+        <v>335</v>
+      </c>
+      <c r="M7" t="s">
+        <v>336</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>744</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>750</v>
+      </c>
+      <c r="P7" t="s">
+        <v>746</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>747</v>
+      </c>
+      <c r="R7" t="s">
+        <v>748</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>745</v>
+      </c>
+      <c r="T7" t="s">
+        <v>749</v>
+      </c>
+      <c r="U7" s="22" t="s">
+        <v>683</v>
+      </c>
+      <c r="V7" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="W7" s="23" t="s">
+        <v>683</v>
+      </c>
+      <c r="X7" s="13" t="s">
+        <v>763</v>
+      </c>
+      <c r="Y7" s="3" t="s">
+        <v>764</v>
+      </c>
+      <c r="Z7" s="14" t="s">
+        <v>752</v>
+      </c>
+      <c r="AA7" s="14" t="s">
+        <v>765</v>
+      </c>
+      <c r="AB7" s="13" t="s">
+        <v>766</v>
+      </c>
+      <c r="AC7" s="13" t="s">
+        <v>767</v>
+      </c>
+      <c r="AD7" s="13" t="s">
+        <v>768</v>
+      </c>
+      <c r="AE7" s="13" t="s">
+        <v>749</v>
+      </c>
+      <c r="AF7" s="14" t="s">
+        <v>769</v>
+      </c>
+      <c r="AG7" s="13" t="s">
+        <v>1040</v>
+      </c>
+      <c r="AH7" s="35" t="s">
+        <v>785</v>
+      </c>
+      <c r="AI7" s="14" t="s">
+        <v>786</v>
+      </c>
+      <c r="AJ7" s="5" t="s">
+        <v>562</v>
+      </c>
+      <c r="AK7" s="5" t="s">
+        <v>787</v>
+      </c>
+      <c r="AL7" t="s">
+        <v>788</v>
+      </c>
+      <c r="AM7" s="2" t="s">
+        <v>789</v>
+      </c>
+      <c r="AN7" s="2" t="s">
+        <v>790</v>
+      </c>
+      <c r="AO7" s="2" t="s">
+        <v>791</v>
+      </c>
+      <c r="AP7" t="s">
+        <v>792</v>
+      </c>
+      <c r="AQ7" t="s">
+        <v>793</v>
+      </c>
+      <c r="AR7" t="s">
+        <v>794</v>
+      </c>
+      <c r="AS7" t="s">
+        <v>795</v>
+      </c>
+      <c r="AT7" s="2" t="s">
+        <v>796</v>
+      </c>
+      <c r="AU7" s="5" t="s">
+        <v>798</v>
+      </c>
+      <c r="AV7" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="AW7" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="AX7" s="5" t="s">
+        <v>814</v>
+      </c>
+      <c r="AY7" s="5" t="s">
+        <v>815</v>
+      </c>
+      <c r="AZ7" s="5" t="s">
+        <v>813</v>
+      </c>
+      <c r="BA7" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="BB7" s="13" t="s">
+        <v>970</v>
+      </c>
+      <c r="BC7" s="13" t="s">
+        <v>971</v>
+      </c>
+      <c r="BD7" s="14" t="s">
+        <v>407</v>
+      </c>
+      <c r="BE7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="BF7" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="BG7" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="BH7" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="BI7" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="BJ7" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="BK7" s="16" t="s">
+        <v>753</v>
+      </c>
+      <c r="BL7" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="BM7" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="BN7" t="s">
+        <v>335</v>
+      </c>
+      <c r="BO7" s="2" t="s">
+        <v>870</v>
+      </c>
+      <c r="BP7" s="2" t="s">
+        <v>870</v>
+      </c>
+      <c r="BQ7" s="2" t="s">
+        <v>873</v>
+      </c>
+      <c r="BR7" s="2" t="s">
+        <v>873</v>
+      </c>
+      <c r="BS7" s="5" t="s">
+        <v>871</v>
+      </c>
+      <c r="BT7" s="5" t="s">
+        <v>872</v>
+      </c>
+      <c r="BU7" s="5" t="s">
+        <v>977</v>
+      </c>
+      <c r="BV7" s="5" t="s">
+        <v>978</v>
+      </c>
+      <c r="BX7" s="5" t="s">
         <v>1035</v>
       </c>
-      <c r="BY6" s="5" t="s">
+      <c r="BY7" s="5" t="s">
         <v>114</v>
+      </c>
+      <c r="CA7" s="5" t="s">
+        <v>969</v>
+      </c>
+      <c r="CB7" s="5" t="s">
+        <v>973</v>
       </c>
     </row>
   </sheetData>
@@ -14335,30 +14649,35 @@
     <hyperlink ref="Y2" r:id="rId1" xr:uid="{784DB924-73E6-40D5-A775-72695CCBC71F}"/>
     <hyperlink ref="AH2" r:id="rId2" xr:uid="{17725C9D-3CB8-4DB2-97DE-D37668DDC8E6}"/>
     <hyperlink ref="BE2" r:id="rId3" xr:uid="{B82E7283-1331-4A52-A31A-1D40CAD29545}"/>
-    <hyperlink ref="Y3" r:id="rId4" xr:uid="{FFEB5818-75A9-4699-AD26-B79EC6D85205}"/>
-    <hyperlink ref="AH3" r:id="rId5" xr:uid="{740A8C71-84AD-41A6-A196-3C9E4A223D19}"/>
-    <hyperlink ref="BE3" r:id="rId6" xr:uid="{8AE534A4-CEF0-4804-98A5-7716AAF65D32}"/>
-    <hyperlink ref="D3" r:id="rId7" xr:uid="{4A613B4A-D536-4E0E-98D5-BC5559D96A95}"/>
+    <hyperlink ref="Y4" r:id="rId4" xr:uid="{FFEB5818-75A9-4699-AD26-B79EC6D85205}"/>
+    <hyperlink ref="AH4" r:id="rId5" xr:uid="{740A8C71-84AD-41A6-A196-3C9E4A223D19}"/>
+    <hyperlink ref="BE4" r:id="rId6" xr:uid="{8AE534A4-CEF0-4804-98A5-7716AAF65D32}"/>
+    <hyperlink ref="D4" r:id="rId7" xr:uid="{4A613B4A-D536-4E0E-98D5-BC5559D96A95}"/>
     <hyperlink ref="E2" r:id="rId8" xr:uid="{3665C397-D83E-4DE6-B006-3127AC277539}"/>
     <hyperlink ref="D2" r:id="rId9" xr:uid="{2E93C007-EFEA-493B-8191-97CAE16ECBB3}"/>
-    <hyperlink ref="Y4" r:id="rId10" xr:uid="{87B53982-2C1D-4D88-9ACA-27DBF403976C}"/>
-    <hyperlink ref="AH4" r:id="rId11" xr:uid="{68FBE87E-FDA5-432F-864A-88887199EF83}"/>
-    <hyperlink ref="BE4" r:id="rId12" xr:uid="{FAFAC8CB-4973-436E-BE47-8CE6694B1553}"/>
-    <hyperlink ref="E4" r:id="rId13" xr:uid="{8ED3696F-04C3-444A-B878-EC9C5EE5361A}"/>
-    <hyperlink ref="Y5" r:id="rId14" xr:uid="{C66E7905-8074-4F50-8B39-CEB08F8BF2BE}"/>
-    <hyperlink ref="AH5" r:id="rId15" xr:uid="{459F1E32-4691-4091-A4D7-B11DDDE61615}"/>
-    <hyperlink ref="BE5" r:id="rId16" xr:uid="{FEABC513-683B-4FB7-B330-639CE56E8E8A}"/>
-    <hyperlink ref="E5" r:id="rId17" xr:uid="{C8AE9799-3A67-4A11-A1B7-592C748F2A34}"/>
-    <hyperlink ref="D5" r:id="rId18" xr:uid="{C2B308A4-E4BC-4D85-9C24-1186C05515C4}"/>
-    <hyperlink ref="Y6" r:id="rId19" xr:uid="{E8ED9264-DE11-4321-9349-7FB21AD7F779}"/>
-    <hyperlink ref="AH6" r:id="rId20" xr:uid="{FCA4A455-4114-4CE5-8F9C-5C35D372AA3A}"/>
-    <hyperlink ref="BE6" r:id="rId21" xr:uid="{CD21D3B5-4FBE-4089-85AB-799407F5E806}"/>
-    <hyperlink ref="E6" r:id="rId22" xr:uid="{8C212082-C529-447B-AE4C-2B3AF19B5A20}"/>
-    <hyperlink ref="D6" r:id="rId23" xr:uid="{0BE74C2F-A572-4D09-AD9F-72932FAD16D8}"/>
-    <hyperlink ref="D4" r:id="rId24" xr:uid="{12046D33-F92A-4149-AA09-13A43CB2CB33}"/>
+    <hyperlink ref="Y5" r:id="rId10" xr:uid="{87B53982-2C1D-4D88-9ACA-27DBF403976C}"/>
+    <hyperlink ref="AH5" r:id="rId11" xr:uid="{68FBE87E-FDA5-432F-864A-88887199EF83}"/>
+    <hyperlink ref="BE5" r:id="rId12" xr:uid="{FAFAC8CB-4973-436E-BE47-8CE6694B1553}"/>
+    <hyperlink ref="E5" r:id="rId13" xr:uid="{8ED3696F-04C3-444A-B878-EC9C5EE5361A}"/>
+    <hyperlink ref="Y6" r:id="rId14" xr:uid="{C66E7905-8074-4F50-8B39-CEB08F8BF2BE}"/>
+    <hyperlink ref="AH6" r:id="rId15" xr:uid="{459F1E32-4691-4091-A4D7-B11DDDE61615}"/>
+    <hyperlink ref="BE6" r:id="rId16" xr:uid="{FEABC513-683B-4FB7-B330-639CE56E8E8A}"/>
+    <hyperlink ref="E6" r:id="rId17" xr:uid="{C8AE9799-3A67-4A11-A1B7-592C748F2A34}"/>
+    <hyperlink ref="D6" r:id="rId18" xr:uid="{C2B308A4-E4BC-4D85-9C24-1186C05515C4}"/>
+    <hyperlink ref="Y7" r:id="rId19" xr:uid="{E8ED9264-DE11-4321-9349-7FB21AD7F779}"/>
+    <hyperlink ref="AH7" r:id="rId20" xr:uid="{FCA4A455-4114-4CE5-8F9C-5C35D372AA3A}"/>
+    <hyperlink ref="BE7" r:id="rId21" xr:uid="{CD21D3B5-4FBE-4089-85AB-799407F5E806}"/>
+    <hyperlink ref="E7" r:id="rId22" xr:uid="{8C212082-C529-447B-AE4C-2B3AF19B5A20}"/>
+    <hyperlink ref="D7" r:id="rId23" xr:uid="{0BE74C2F-A572-4D09-AD9F-72932FAD16D8}"/>
+    <hyperlink ref="D5" r:id="rId24" xr:uid="{12046D33-F92A-4149-AA09-13A43CB2CB33}"/>
+    <hyperlink ref="Y3" r:id="rId25" xr:uid="{B4B982CA-76A5-416C-85C3-42CBD495F0DD}"/>
+    <hyperlink ref="AH3" r:id="rId26" xr:uid="{22315634-AF9B-4D7A-AE14-9A1F69A534F6}"/>
+    <hyperlink ref="BE3" r:id="rId27" xr:uid="{88A4D912-C289-4B12-9636-F2CCCB13ED5C}"/>
+    <hyperlink ref="E3" r:id="rId28" xr:uid="{0FB16AFA-38E8-4F48-999D-915A68E01F3E}"/>
+    <hyperlink ref="D3" r:id="rId29" xr:uid="{33A495B0-32F7-4EB6-8838-7C0ED697FD35}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId25"/>
+  <pageSetup orientation="portrait" r:id="rId30"/>
 </worksheet>
 </file>
 
@@ -15207,7 +15526,7 @@
         <v>1001</v>
       </c>
       <c r="AC1" s="21" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="AD1" s="21" t="s">
         <v>728</v>
@@ -15231,7 +15550,7 @@
         <v>832</v>
       </c>
       <c r="AK1" s="8" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="AL1" s="8" t="s">
         <v>837</v>
@@ -15291,13 +15610,13 @@
         <v>1010</v>
       </c>
       <c r="BE1" s="8" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="BF1" s="8" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="BG1" s="8" t="s">
-        <v>1108</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="2" spans="1:59">
@@ -15576,7 +15895,7 @@
         <v>335</v>
       </c>
       <c r="M5" s="24" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="N5" s="33" t="s">
         <v>635</v>
@@ -15656,7 +15975,7 @@
         <v>335</v>
       </c>
       <c r="M6" s="24" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="N6" s="33" t="s">
         <v>635</v>
@@ -15784,7 +16103,7 @@
         <v>825</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="C8" s="24" t="s">
         <v>22</v>
@@ -15906,7 +16225,7 @@
       <c r="AG9" s="5"/>
       <c r="AH9" s="5"/>
       <c r="BG9" s="48" t="s">
-        <v>1109</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="10" spans="1:59">
@@ -17350,7 +17669,7 @@
         <v>916</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="C30" s="24" t="s">
         <v>22</v>
@@ -17841,7 +18160,7 @@
         <v>22</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>24</v>
@@ -17943,7 +18262,7 @@
         <v>42</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>24</v>
@@ -18516,13 +18835,13 @@
         <v>843</v>
       </c>
       <c r="B45" s="22" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="C45" s="24" t="s">
         <v>22</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>24</v>
@@ -18623,10 +18942,10 @@
     </row>
     <row r="47" spans="1:58">
       <c r="A47" s="22" t="s">
+        <v>1087</v>
+      </c>
+      <c r="B47" s="22" t="s">
         <v>1088</v>
-      </c>
-      <c r="B47" s="22" t="s">
-        <v>1089</v>
       </c>
       <c r="C47" s="24" t="s">
         <v>22</v>
@@ -18656,10 +18975,10 @@
         <v>634</v>
       </c>
       <c r="L47" s="22" t="s">
+        <v>1091</v>
+      </c>
+      <c r="M47" s="24" t="s">
         <v>1092</v>
-      </c>
-      <c r="M47" s="24" t="s">
-        <v>1093</v>
       </c>
       <c r="N47" s="33" t="s">
         <v>635</v>
@@ -18671,10 +18990,10 @@
         <v>994</v>
       </c>
       <c r="BE47" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="BF47" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
     </row>
   </sheetData>
@@ -19358,10 +19677,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65BCC974-80FA-4619-98C6-71D6CDC1F642}">
-  <dimension ref="A1:AG12"/>
+  <dimension ref="A1:AI14"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="AH7" sqref="AH7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -19375,6 +19694,7 @@
     <col min="7" max="7" width="15.140625" customWidth="1"/>
     <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.85546875" customWidth="1"/>
     <col min="14" max="14" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="16.28515625" customWidth="1"/>
@@ -19382,9 +19702,11 @@
     <col min="30" max="30" width="23.42578125" customWidth="1"/>
     <col min="31" max="31" width="21.42578125" customWidth="1"/>
     <col min="32" max="32" width="14.28515625" customWidth="1"/>
+    <col min="34" max="34" width="18.28515625" customWidth="1"/>
+    <col min="35" max="35" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33">
+    <row r="1" spans="1:35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -19482,8 +19804,14 @@
       <c r="AG1" s="8" t="s">
         <v>699</v>
       </c>
-    </row>
-    <row r="2" spans="1:33">
+      <c r="AH1" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="AI1" s="8" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35">
       <c r="A2" s="22" t="s">
         <v>874</v>
       </c>
@@ -19538,7 +19866,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="3" spans="1:33">
+    <row r="3" spans="1:35">
       <c r="A3" s="22" t="s">
         <v>875</v>
       </c>
@@ -19595,7 +19923,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="4" spans="1:33">
+    <row r="4" spans="1:35">
       <c r="A4" s="22" t="s">
         <v>875</v>
       </c>
@@ -19650,7 +19978,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="5" spans="1:33">
+    <row r="5" spans="1:35">
       <c r="A5" s="22" t="s">
         <v>875</v>
       </c>
@@ -19705,27 +20033,27 @@
         <v>332</v>
       </c>
     </row>
-    <row r="6" spans="1:33" ht="16.5">
+    <row r="6" spans="1:35">
       <c r="A6" s="22" t="s">
-        <v>157</v>
+        <v>875</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>691</v>
+        <v>1115</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" s="24" t="s">
-        <v>31</v>
-      </c>
+        <v>1116</v>
+      </c>
+      <c r="F6" s="22"/>
       <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
+      <c r="H6" s="22" t="s">
+        <v>1117</v>
+      </c>
       <c r="I6" s="22"/>
       <c r="J6" s="22"/>
       <c r="K6" s="22"/>
@@ -19734,9 +20062,7 @@
       <c r="N6" t="s">
         <v>332</v>
       </c>
-      <c r="O6" s="23" t="s">
-        <v>158</v>
-      </c>
+      <c r="O6" s="22"/>
       <c r="P6" s="22"/>
       <c r="Q6" s="22"/>
       <c r="R6" s="22"/>
@@ -19749,16 +20075,9 @@
       </c>
       <c r="V6" s="22"/>
       <c r="W6" s="22"/>
-      <c r="X6" s="19" t="s">
-        <v>105</v>
-      </c>
-      <c r="Y6" s="23" t="s">
-        <v>159</v>
-      </c>
-      <c r="Z6" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="AB6" s="5"/>
+      <c r="X6" s="22"/>
+      <c r="Y6" s="22"/>
+      <c r="Z6" s="22"/>
       <c r="AD6" s="5" t="s">
         <v>969</v>
       </c>
@@ -19768,16 +20087,13 @@
       <c r="AF6" t="s">
         <v>332</v>
       </c>
-      <c r="AG6" s="5" t="s">
-        <v>717</v>
-      </c>
-    </row>
-    <row r="7" spans="1:33" ht="16.5">
+    </row>
+    <row r="7" spans="1:35">
       <c r="A7" s="22" t="s">
-        <v>160</v>
+        <v>1118</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>689</v>
+        <v>1119</v>
       </c>
       <c r="C7" s="24" t="s">
         <v>22</v>
@@ -19788,9 +20104,7 @@
       <c r="E7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="24" t="s">
-        <v>31</v>
-      </c>
+      <c r="F7" s="22"/>
       <c r="G7" s="22"/>
       <c r="H7" s="22"/>
       <c r="I7" s="22"/>
@@ -19798,59 +20112,36 @@
       <c r="K7" s="22"/>
       <c r="L7" s="22"/>
       <c r="M7" s="22"/>
-      <c r="N7" t="s">
-        <v>332</v>
-      </c>
-      <c r="O7" s="23" t="s">
-        <v>158</v>
-      </c>
+      <c r="O7" s="22"/>
       <c r="P7" s="22"/>
       <c r="Q7" s="22"/>
       <c r="R7" s="22"/>
       <c r="S7" s="22"/>
-      <c r="T7" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="U7" s="5" t="s">
-        <v>32</v>
-      </c>
+      <c r="T7" s="5"/>
+      <c r="U7" s="5"/>
       <c r="V7" s="22"/>
       <c r="W7" s="22"/>
-      <c r="X7" s="19" t="s">
-        <v>105</v>
-      </c>
-      <c r="Y7" s="23" t="s">
-        <v>159</v>
-      </c>
+      <c r="X7" s="22"/>
+      <c r="Y7" s="22"/>
       <c r="Z7" s="22"/>
-      <c r="AA7" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="AB7" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="AC7" t="s">
-        <v>127</v>
-      </c>
-      <c r="AD7" s="5" t="s">
-        <v>969</v>
-      </c>
-      <c r="AE7" s="5" t="s">
-        <v>973</v>
-      </c>
-      <c r="AF7" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="8" spans="1:33" ht="16.5">
+      <c r="AD7" s="5"/>
+      <c r="AE7" s="5"/>
+      <c r="AH7" t="s">
+        <v>1121</v>
+      </c>
+      <c r="AI7" s="3" t="s">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:35" ht="16.5">
       <c r="A8" s="22" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>23</v>
@@ -19878,19 +20169,24 @@
       <c r="Q8" s="22"/>
       <c r="R8" s="22"/>
       <c r="S8" s="22"/>
-      <c r="T8" s="5"/>
-      <c r="U8" s="5"/>
+      <c r="T8" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="U8" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="V8" s="22"/>
       <c r="W8" s="22"/>
-      <c r="X8" s="19"/>
-      <c r="Y8" s="23"/>
-      <c r="Z8" s="22"/>
-      <c r="AA8" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="AB8" s="5" t="s">
-        <v>126</v>
-      </c>
+      <c r="X8" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="Y8" s="23" t="s">
+        <v>159</v>
+      </c>
+      <c r="Z8" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB8" s="5"/>
       <c r="AD8" s="5" t="s">
         <v>969</v>
       </c>
@@ -19900,13 +20196,16 @@
       <c r="AF8" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="9" spans="1:33" ht="16.5">
+      <c r="AG8" s="5" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="9" spans="1:35" ht="16.5">
       <c r="A9" s="22" t="s">
-        <v>1100</v>
+        <v>160</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>1100</v>
+        <v>689</v>
       </c>
       <c r="C9" s="24" t="s">
         <v>22</v>
@@ -19930,7 +20229,9 @@
       <c r="N9" t="s">
         <v>332</v>
       </c>
-      <c r="O9" s="22"/>
+      <c r="O9" s="23" t="s">
+        <v>158</v>
+      </c>
       <c r="P9" s="22"/>
       <c r="Q9" s="22"/>
       <c r="R9" s="22"/>
@@ -19946,8 +20247,19 @@
       <c r="X9" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="Y9" s="22"/>
+      <c r="Y9" s="23" t="s">
+        <v>159</v>
+      </c>
       <c r="Z9" s="22"/>
+      <c r="AA9" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="AB9" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>127</v>
+      </c>
       <c r="AD9" s="5" t="s">
         <v>969</v>
       </c>
@@ -19958,15 +20270,15 @@
         <v>332</v>
       </c>
     </row>
-    <row r="10" spans="1:33" ht="16.5">
+    <row r="10" spans="1:35" ht="16.5">
       <c r="A10" s="22" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>162</v>
+        <v>690</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>23</v>
@@ -19994,22 +20306,18 @@
       <c r="Q10" s="22"/>
       <c r="R10" s="22"/>
       <c r="S10" s="22"/>
-      <c r="T10" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="U10" s="5" t="s">
-        <v>32</v>
-      </c>
+      <c r="T10" s="5"/>
+      <c r="U10" s="5"/>
       <c r="V10" s="22"/>
       <c r="W10" s="22"/>
-      <c r="X10" s="19" t="s">
-        <v>105</v>
-      </c>
-      <c r="Y10" s="23" t="s">
-        <v>159</v>
-      </c>
-      <c r="Z10" s="24" t="s">
-        <v>34</v>
+      <c r="X10" s="19"/>
+      <c r="Y10" s="23"/>
+      <c r="Z10" s="22"/>
+      <c r="AA10" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="AB10" s="5" t="s">
+        <v>126</v>
       </c>
       <c r="AD10" s="5" t="s">
         <v>969</v>
@@ -20021,25 +20329,53 @@
         <v>332</v>
       </c>
     </row>
-    <row r="11" spans="1:33" ht="210">
-      <c r="A11" t="s">
-        <v>709</v>
+    <row r="11" spans="1:35" ht="16.5">
+      <c r="A11" s="22" t="s">
+        <v>1098</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>710</v>
+        <v>1098</v>
       </c>
       <c r="C11" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="43" t="s">
-        <v>935</v>
-      </c>
-      <c r="E11" s="44" t="s">
-        <v>985</v>
-      </c>
+      <c r="D11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="22"/>
+      <c r="M11" s="22"/>
       <c r="N11" t="s">
         <v>332</v>
       </c>
+      <c r="O11" s="22"/>
+      <c r="P11" s="22"/>
+      <c r="Q11" s="22"/>
+      <c r="R11" s="22"/>
+      <c r="S11" s="22"/>
+      <c r="T11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="U11" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="V11" s="22"/>
+      <c r="W11" s="22"/>
+      <c r="X11" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="Y11" s="22"/>
+      <c r="Z11" s="22"/>
       <c r="AD11" s="5" t="s">
         <v>969</v>
       </c>
@@ -20050,12 +20386,12 @@
         <v>332</v>
       </c>
     </row>
-    <row r="12" spans="1:33">
+    <row r="12" spans="1:35" ht="16.5">
       <c r="A12" s="22" t="s">
-        <v>974</v>
+        <v>161</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>974</v>
+        <v>162</v>
       </c>
       <c r="C12" s="24" t="s">
         <v>22</v>
@@ -20069,8 +20405,39 @@
       <c r="F12" s="24" t="s">
         <v>31</v>
       </c>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="22"/>
+      <c r="L12" s="22"/>
+      <c r="M12" s="22"/>
       <c r="N12" t="s">
         <v>332</v>
+      </c>
+      <c r="O12" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="P12" s="22"/>
+      <c r="Q12" s="22"/>
+      <c r="R12" s="22"/>
+      <c r="S12" s="22"/>
+      <c r="T12" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="U12" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="V12" s="22"/>
+      <c r="W12" s="22"/>
+      <c r="X12" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="Y12" s="23" t="s">
+        <v>159</v>
+      </c>
+      <c r="Z12" s="24" t="s">
+        <v>34</v>
       </c>
       <c r="AD12" s="5" t="s">
         <v>969</v>
@@ -20079,6 +20446,67 @@
         <v>973</v>
       </c>
       <c r="AF12" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="13" spans="1:35" ht="210">
+      <c r="A13" t="s">
+        <v>709</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>710</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="43" t="s">
+        <v>935</v>
+      </c>
+      <c r="E13" s="44" t="s">
+        <v>985</v>
+      </c>
+      <c r="N13" t="s">
+        <v>332</v>
+      </c>
+      <c r="AD13" s="5" t="s">
+        <v>969</v>
+      </c>
+      <c r="AE13" s="5" t="s">
+        <v>973</v>
+      </c>
+      <c r="AF13" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="14" spans="1:35">
+      <c r="A14" s="22" t="s">
+        <v>974</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>974</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="N14" t="s">
+        <v>332</v>
+      </c>
+      <c r="AD14" s="5" t="s">
+        <v>969</v>
+      </c>
+      <c r="AE14" s="5" t="s">
+        <v>973</v>
+      </c>
+      <c r="AF14" t="s">
         <v>332</v>
       </c>
     </row>
@@ -20087,21 +20515,24 @@
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1" display="bicipat748@topyte.com" xr:uid="{FE80212F-06E6-4EDC-A56B-C70DE7430F0D}"/>
     <hyperlink ref="E5" r:id="rId2" xr:uid="{A474C459-AC63-4F79-B8AC-E155C931F790}"/>
-    <hyperlink ref="E6" r:id="rId3" xr:uid="{9425CF72-71E3-44FF-A0A4-C2379FB8BCBC}"/>
-    <hyperlink ref="E7" r:id="rId4" xr:uid="{6A25299C-16CA-4569-AB0E-13B84A957550}"/>
-    <hyperlink ref="E9" r:id="rId5" xr:uid="{6B7BC84F-1875-416C-892F-19DDE04ACFBF}"/>
-    <hyperlink ref="E10" r:id="rId6" xr:uid="{2828F4A3-1950-4B34-A9FB-0639E65F5F8D}"/>
+    <hyperlink ref="E8" r:id="rId3" xr:uid="{9425CF72-71E3-44FF-A0A4-C2379FB8BCBC}"/>
+    <hyperlink ref="E9" r:id="rId4" xr:uid="{6A25299C-16CA-4569-AB0E-13B84A957550}"/>
+    <hyperlink ref="E11" r:id="rId5" xr:uid="{6B7BC84F-1875-416C-892F-19DDE04ACFBF}"/>
+    <hyperlink ref="E12" r:id="rId6" xr:uid="{2828F4A3-1950-4B34-A9FB-0639E65F5F8D}"/>
     <hyperlink ref="D4" r:id="rId7" xr:uid="{A68155FA-92C4-46EE-A6EC-4CBA185C461F}"/>
     <hyperlink ref="E4" r:id="rId8" display="mailto:Admin@123" xr:uid="{6770697B-7990-4F65-AD1D-8B3C52F0019A}"/>
-    <hyperlink ref="E8" r:id="rId9" xr:uid="{54305EEA-208F-4DEF-B680-E8EC95C88152}"/>
+    <hyperlink ref="E10" r:id="rId9" xr:uid="{54305EEA-208F-4DEF-B680-E8EC95C88152}"/>
     <hyperlink ref="E3" r:id="rId10" display="mailto:Admin@123" xr:uid="{C96FBEFA-945F-4D81-8620-EEED20AAEB31}"/>
-    <hyperlink ref="E12" r:id="rId11" xr:uid="{D685B2E7-66D2-46EA-948C-672B94FAAE1F}"/>
+    <hyperlink ref="E14" r:id="rId11" xr:uid="{D685B2E7-66D2-46EA-948C-672B94FAAE1F}"/>
     <hyperlink ref="E2" r:id="rId12" xr:uid="{95D49E27-2840-406A-8D46-11DC27F5A8BC}"/>
     <hyperlink ref="D2" r:id="rId13" xr:uid="{BACA1E63-2785-4A82-A112-FFD0158A117F}"/>
-    <hyperlink ref="E11" r:id="rId14" xr:uid="{93B2FF03-2485-4EB6-98F4-FCD0ACA0539A}"/>
+    <hyperlink ref="E13" r:id="rId14" xr:uid="{93B2FF03-2485-4EB6-98F4-FCD0ACA0539A}"/>
+    <hyperlink ref="E6" r:id="rId15" xr:uid="{0078A3C7-A908-4306-BA3F-3ADC17E1F2D7}"/>
+    <hyperlink ref="AI7" r:id="rId16" xr:uid="{92F3C8F3-2F2D-4F31-81B4-79DD035C7061}"/>
+    <hyperlink ref="E7" r:id="rId17" xr:uid="{B0843AE4-E904-4EB0-9C71-2E6DC74D8652}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId15"/>
+  <pageSetup orientation="portrait" r:id="rId18"/>
 </worksheet>
 </file>
 
@@ -20671,8 +21102,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13349954-3C44-451A-AD0B-7C1C97C692A7}">
   <dimension ref="A1:AA24"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView topLeftCell="S1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Y24" sqref="Y24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -21785,8 +22216,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CD6D202-32E3-4E97-B778-6720B640BBA7}">
   <dimension ref="A1:AU36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="U21" sqref="U21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -21962,7 +22393,7 @@
         <v>961</v>
       </c>
       <c r="AS1" s="8" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="AT1" s="1" t="s">
         <v>713</v>
@@ -22170,7 +22601,7 @@
         <v>1050</v>
       </c>
       <c r="V6" s="40" t="s">
-        <v>1051</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="7" spans="1:47">
@@ -22220,7 +22651,7 @@
         <v>1050</v>
       </c>
       <c r="V7" s="40" t="s">
-        <v>1051</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="8" spans="1:47">
@@ -22270,7 +22701,7 @@
         <v>1050</v>
       </c>
       <c r="V8" s="40" t="s">
-        <v>1051</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="9" spans="1:47">
@@ -22316,7 +22747,7 @@
         <v>1050</v>
       </c>
       <c r="V9" s="40" t="s">
-        <v>1051</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="10" spans="1:47">
@@ -22362,7 +22793,7 @@
         <v>1050</v>
       </c>
       <c r="V10" s="40" t="s">
-        <v>1051</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="11" spans="1:47">
@@ -22408,7 +22839,7 @@
         <v>1050</v>
       </c>
       <c r="V11" s="40" t="s">
-        <v>1051</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="12" spans="1:47">
@@ -22661,7 +23092,7 @@
         <v>1050</v>
       </c>
       <c r="V17" s="40" t="s">
-        <v>1051</v>
+        <v>1109</v>
       </c>
       <c r="W17" s="5" t="s">
         <v>256</v>
@@ -22795,7 +23226,7 @@
         <v>1050</v>
       </c>
       <c r="V20" s="40" t="s">
-        <v>1051</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="21" spans="1:44">
@@ -22848,7 +23279,7 @@
         <v>1050</v>
       </c>
       <c r="V21" s="40" t="s">
-        <v>1051</v>
+        <v>1109</v>
       </c>
       <c r="Z21" s="5" t="s">
         <v>263</v>
@@ -22937,7 +23368,7 @@
         <v>1050</v>
       </c>
       <c r="V22" s="40" t="s">
-        <v>1051</v>
+        <v>1109</v>
       </c>
       <c r="Z22" s="5" t="s">
         <v>263</v>
@@ -23026,7 +23457,7 @@
         <v>1050</v>
       </c>
       <c r="V23" s="40" t="s">
-        <v>1051</v>
+        <v>1109</v>
       </c>
       <c r="Z23" s="5" t="s">
         <v>263</v>
@@ -23112,7 +23543,7 @@
         <v>1050</v>
       </c>
       <c r="V24" s="40" t="s">
-        <v>1051</v>
+        <v>1109</v>
       </c>
       <c r="Z24" s="5"/>
       <c r="AJ24" s="27" t="s">
@@ -23169,7 +23600,7 @@
         <v>1050</v>
       </c>
       <c r="V25" s="40" t="s">
-        <v>1051</v>
+        <v>1109</v>
       </c>
       <c r="Z25" s="5" t="s">
         <v>263</v>
@@ -23255,7 +23686,7 @@
         <v>1050</v>
       </c>
       <c r="V26" s="40" t="s">
-        <v>1051</v>
+        <v>1109</v>
       </c>
       <c r="Z26" s="5" t="s">
         <v>263</v>
@@ -23328,7 +23759,7 @@
         <v>1050</v>
       </c>
       <c r="V27" s="40" t="s">
-        <v>1051</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="28" spans="1:44">
@@ -23378,7 +23809,7 @@
         <v>1050</v>
       </c>
       <c r="V28" s="40" t="s">
-        <v>1051</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="29" spans="1:44">
@@ -23428,7 +23859,7 @@
         <v>1050</v>
       </c>
       <c r="V29" s="40" t="s">
-        <v>1051</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="30" spans="1:44">
@@ -23436,7 +23867,7 @@
         <v>274</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="C30" s="24" t="s">
         <v>48</v>
@@ -23466,7 +23897,7 @@
         <v>260</v>
       </c>
       <c r="P30" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="R30" s="2" t="s">
         <v>262</v>
@@ -23478,7 +23909,7 @@
         <v>1050</v>
       </c>
       <c r="V30" s="40" t="s">
-        <v>1051</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="31" spans="1:44">
@@ -23486,7 +23917,7 @@
         <v>274</v>
       </c>
       <c r="B31" s="22" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="C31" s="24" t="s">
         <v>51</v>
@@ -23516,7 +23947,7 @@
         <v>260</v>
       </c>
       <c r="P31" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="R31" s="2" t="s">
         <v>262</v>
@@ -23528,7 +23959,7 @@
         <v>1050</v>
       </c>
       <c r="V31" s="40" t="s">
-        <v>1051</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="32" spans="1:44">
@@ -23644,10 +24075,10 @@
     </row>
     <row r="35" spans="1:47">
       <c r="A35" s="22" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="B35" s="22" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>22</v>
@@ -23671,15 +24102,15 @@
         <v>332</v>
       </c>
       <c r="AS35" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="36" spans="1:47">
       <c r="A36" t="s">
-        <v>1110</v>
+        <v>1108</v>
       </c>
       <c r="B36" s="22" t="s">
-        <v>1107</v>
+        <v>1105</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>22</v>
@@ -23771,8 +24202,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE239896-844A-4CCC-92E6-4B83AF52C480}">
   <dimension ref="A1:AB15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -23936,10 +24367,10 @@
         <v>295</v>
       </c>
       <c r="R2" s="40" t="s">
-        <v>1050</v>
+        <v>1123</v>
       </c>
       <c r="S2" s="40" t="s">
-        <v>1051</v>
+        <v>1122</v>
       </c>
       <c r="T2" s="5" t="s">
         <v>260</v>
@@ -23998,10 +24429,10 @@
         <v>295</v>
       </c>
       <c r="R3" s="40" t="s">
-        <v>1050</v>
+        <v>1123</v>
       </c>
       <c r="S3" s="40" t="s">
-        <v>1051</v>
+        <v>1122</v>
       </c>
       <c r="T3" s="5" t="s">
         <v>260</v>
@@ -24060,10 +24491,10 @@
         <v>295</v>
       </c>
       <c r="R4" s="40" t="s">
-        <v>1050</v>
+        <v>1123</v>
       </c>
       <c r="S4" s="40" t="s">
-        <v>1051</v>
+        <v>1122</v>
       </c>
       <c r="T4" s="5" t="s">
         <v>260</v>
@@ -24119,10 +24550,10 @@
         <v>295</v>
       </c>
       <c r="R5" s="40" t="s">
-        <v>1050</v>
+        <v>1123</v>
       </c>
       <c r="S5" s="40" t="s">
-        <v>1051</v>
+        <v>1122</v>
       </c>
       <c r="T5" s="5" t="s">
         <v>260</v>
@@ -24181,10 +24612,10 @@
         <v>295</v>
       </c>
       <c r="R6" s="40" t="s">
-        <v>1050</v>
+        <v>1123</v>
       </c>
       <c r="S6" s="40" t="s">
-        <v>1051</v>
+        <v>1122</v>
       </c>
       <c r="T6" s="5" t="s">
         <v>260</v>
@@ -24243,10 +24674,10 @@
         <v>295</v>
       </c>
       <c r="R7" s="40" t="s">
-        <v>1050</v>
+        <v>1123</v>
       </c>
       <c r="S7" s="40" t="s">
-        <v>1051</v>
+        <v>1122</v>
       </c>
       <c r="T7" s="5" t="s">
         <v>260</v>
@@ -24305,10 +24736,10 @@
         <v>295</v>
       </c>
       <c r="R8" s="40" t="s">
-        <v>1050</v>
+        <v>1123</v>
       </c>
       <c r="S8" s="40" t="s">
-        <v>1051</v>
+        <v>1122</v>
       </c>
       <c r="T8" s="5" t="s">
         <v>260</v>
@@ -24370,10 +24801,10 @@
         <v>295</v>
       </c>
       <c r="R9" s="40" t="s">
-        <v>1050</v>
+        <v>1123</v>
       </c>
       <c r="S9" s="40" t="s">
-        <v>1051</v>
+        <v>1122</v>
       </c>
       <c r="T9" s="5" t="s">
         <v>260</v>
@@ -24438,10 +24869,10 @@
         <v>295</v>
       </c>
       <c r="R10" s="40" t="s">
-        <v>1050</v>
+        <v>1123</v>
       </c>
       <c r="S10" s="40" t="s">
-        <v>1051</v>
+        <v>1122</v>
       </c>
       <c r="T10" s="5" t="s">
         <v>260</v>
@@ -24506,10 +24937,10 @@
         <v>295</v>
       </c>
       <c r="R11" s="40" t="s">
-        <v>1050</v>
+        <v>1123</v>
       </c>
       <c r="S11" s="40" t="s">
-        <v>1051</v>
+        <v>1122</v>
       </c>
       <c r="T11" s="5" t="s">
         <v>260</v>
@@ -24586,10 +25017,10 @@
         <v>295</v>
       </c>
       <c r="R12" s="40" t="s">
-        <v>1050</v>
+        <v>1123</v>
       </c>
       <c r="S12" s="40" t="s">
-        <v>1051</v>
+        <v>1122</v>
       </c>
       <c r="T12" s="5" t="s">
         <v>260</v>
@@ -24966,7 +25397,7 @@
         <v>337</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>1099</v>
+        <v>1097</v>
       </c>
       <c r="Q2" s="5" t="s">
         <v>339</v>
@@ -26954,10 +27385,10 @@
         <v>334</v>
       </c>
       <c r="M33" s="19" t="s">
-        <v>1101</v>
+        <v>1099</v>
       </c>
       <c r="N33" s="19" t="s">
-        <v>1101</v>
+        <v>1099</v>
       </c>
       <c r="O33" s="3" t="s">
         <v>1021</v>

</xml_diff>